<commit_message>
Calculate equipment billing amounts accurately using unit and rate values
Adds new scripts calculate_pm_allocations.py, direct_billing_extract.py, and preserve_original_amounts.py to generate accurate billing reports.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/85757280-ce77-43c9-81a6-608022a40f5e.jpg
</commit_message>
<xml_diff>
--- a/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
+++ b/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
@@ -5564,7 +5564,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H92" t="n">
@@ -5620,7 +5620,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H93" t="n">
@@ -5680,7 +5680,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -5736,7 +5736,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H95" t="n">
@@ -5796,7 +5796,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H96" t="n">
@@ -5856,7 +5856,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H97" t="n">
@@ -5916,7 +5916,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H98" t="n">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H105" t="n">
@@ -6364,7 +6364,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H106" t="n">
@@ -6420,7 +6420,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H107" t="n">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H108" t="n">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H109" t="n">
@@ -6808,7 +6808,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H114" t="n">
@@ -6972,7 +6972,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H117" t="n">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H118" t="n">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H119" t="n">
@@ -7140,7 +7140,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H120" t="n">
@@ -7200,7 +7200,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M | 9000 100F | CC NEEDED</t>
         </is>
       </c>
       <c r="H121" t="n">
@@ -7256,7 +7256,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M | 9000 100F | CC NEEDED</t>
         </is>
       </c>
       <c r="H122" t="n">
@@ -7312,7 +7312,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100M | 9000 100F | CC NEEDED</t>
         </is>
       </c>
       <c r="H123" t="n">
@@ -7366,7 +7366,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H124" t="n">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H125" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H126" t="n">
@@ -7534,7 +7534,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H127" t="n">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H143" t="n">
@@ -8476,7 +8476,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H144" t="n">
@@ -8532,7 +8532,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H145" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H146" t="n">
@@ -8644,7 +8644,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H147" t="n">
@@ -8700,7 +8700,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H148" t="n">
@@ -8756,7 +8756,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H149" t="n">
@@ -8812,7 +8812,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H150" t="n">
@@ -8868,7 +8868,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H151" t="n">
@@ -8924,7 +8924,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H152" t="n">
@@ -8980,7 +8980,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H153" t="n">
@@ -9036,7 +9036,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H154" t="n">
@@ -9092,7 +9092,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H155" t="n">
@@ -9146,7 +9146,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H156" t="n">
@@ -9202,7 +9202,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H157" t="n">
@@ -9258,7 +9258,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H158" t="n">
@@ -9314,7 +9314,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H159" t="n">
@@ -9368,7 +9368,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H160" t="n">
@@ -9424,7 +9424,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H161" t="n">
@@ -9480,7 +9480,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H162" t="n">
@@ -9536,7 +9536,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H163" t="n">
@@ -9592,7 +9592,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H164" t="n">
@@ -9648,7 +9648,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H165" t="n">
@@ -9704,7 +9704,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H166" t="n">
@@ -9760,7 +9760,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H167" t="n">
@@ -9816,7 +9816,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H168" t="n">
@@ -9872,7 +9872,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H169" t="n">
@@ -9928,7 +9928,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H170" t="n">
@@ -9984,7 +9984,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H171" t="n">
@@ -10040,7 +10040,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H172" t="n">
@@ -10096,7 +10096,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H173" t="n">
@@ -10152,7 +10152,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H174" t="n">
@@ -10208,7 +10208,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H175" t="n">
@@ -10264,7 +10264,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H176" t="n">
@@ -10320,7 +10320,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H177" t="n">
@@ -10376,7 +10376,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H178" t="n">
@@ -10430,7 +10430,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H179" t="n">
@@ -10484,7 +10484,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H180" t="n">
@@ -10538,7 +10538,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H181" t="n">
@@ -10594,7 +10594,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H182" t="n">
@@ -10650,7 +10650,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H183" t="n">
@@ -10706,7 +10706,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H184" t="n">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H185" t="n">
@@ -10818,7 +10818,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H186" t="n">
@@ -10872,7 +10872,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H187" t="n">
@@ -10926,7 +10926,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H188" t="n">
@@ -10980,7 +10980,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H189" t="n">
@@ -11036,7 +11036,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H190" t="n">
@@ -11090,7 +11090,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H191" t="n">
@@ -11146,7 +11146,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H192" t="n">
@@ -11202,7 +11202,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H193" t="n">
@@ -11256,7 +11256,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H194" t="n">
@@ -11310,7 +11310,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H195" t="n">
@@ -11364,7 +11364,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H196" t="n">
@@ -11420,7 +11420,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H197" t="n">
@@ -11476,7 +11476,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H198" t="n">
@@ -11532,7 +11532,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H199" t="n">
@@ -11588,7 +11588,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H200" t="n">
@@ -11644,7 +11644,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H201" t="n">
@@ -11700,7 +11700,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H202" t="n">
@@ -11756,7 +11756,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H203" t="n">
@@ -11812,7 +11812,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H204" t="n">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H205" t="n">
@@ -11922,7 +11922,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H206" t="n">
@@ -11978,7 +11978,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H207" t="n">
@@ -12034,7 +12034,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H208" t="n">
@@ -12090,7 +12090,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H209" t="n">
@@ -12146,7 +12146,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H210" t="n">
@@ -12202,7 +12202,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H211" t="n">
@@ -12258,7 +12258,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H212" t="n">
@@ -12312,7 +12312,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H213" t="n">
@@ -12366,7 +12366,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H214" t="n">
@@ -12420,7 +12420,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H215" t="n">
@@ -12474,7 +12474,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H216" t="n">
@@ -12528,7 +12528,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H217" t="n">
@@ -12582,7 +12582,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H218" t="n">
@@ -12636,7 +12636,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H219" t="n">
@@ -12690,7 +12690,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H220" t="n">
@@ -12744,7 +12744,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H221" t="n">
@@ -12798,7 +12798,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H222" t="n">
@@ -12852,7 +12852,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H223" t="n">
@@ -12906,7 +12906,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H224" t="n">
@@ -12960,7 +12960,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H225" t="n">
@@ -13014,7 +13014,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H226" t="n">
@@ -13068,7 +13068,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H227" t="n">
@@ -13122,7 +13122,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H228" t="n">
@@ -13176,7 +13176,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H229" t="n">
@@ -13230,7 +13230,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H230" t="n">
@@ -13284,7 +13284,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H231" t="n">
@@ -13338,7 +13338,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H232" t="n">
@@ -13392,7 +13392,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H233" t="n">
@@ -13446,7 +13446,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H234" t="n">
@@ -13500,7 +13500,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H235" t="n">
@@ -13556,7 +13556,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H236" t="n">
@@ -13610,7 +13610,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H237" t="n">
@@ -13664,7 +13664,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H238" t="n">
@@ -13718,7 +13718,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H239" t="n">
@@ -13772,7 +13772,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H240" t="n">
@@ -13828,7 +13828,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H241" t="n">
@@ -13882,7 +13882,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H242" t="n">
@@ -13936,7 +13936,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H243" t="n">
@@ -13990,7 +13990,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H244" t="n">
@@ -14044,7 +14044,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H245" t="n">
@@ -14098,7 +14098,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H246" t="n">
@@ -14152,7 +14152,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H247" t="n">
@@ -14206,7 +14206,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H248" t="n">
@@ -14260,7 +14260,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H249" t="n">
@@ -14314,7 +14314,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H250" t="n">
@@ -14368,7 +14368,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H251" t="n">
@@ -14422,7 +14422,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H252" t="n">
@@ -14476,7 +14476,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H253" t="n">
@@ -14530,7 +14530,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H254" t="n">
@@ -14584,7 +14584,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H255" t="n">
@@ -14638,7 +14638,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H256" t="n">
@@ -14692,7 +14692,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H257" t="n">
@@ -14746,7 +14746,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H258" t="n">
@@ -14806,7 +14806,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H259" t="n">
@@ -14862,7 +14862,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H260" t="n">
@@ -14918,7 +14918,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H261" t="n">
@@ -14974,7 +14974,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H262" t="n">
@@ -15030,7 +15030,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H263" t="n">
@@ -15086,7 +15086,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H264" t="n">
@@ -15142,7 +15142,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H265" t="n">
@@ -15196,7 +15196,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H266" t="n">
@@ -15252,7 +15252,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H267" t="n">
@@ -15308,7 +15308,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H268" t="n">
@@ -15362,7 +15362,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H269" t="n">
@@ -15418,7 +15418,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H270" t="n">
@@ -15474,7 +15474,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H271" t="n">
@@ -15530,7 +15530,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H272" t="n">
@@ -15586,7 +15586,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H273" t="n">
@@ -15642,7 +15642,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H274" t="n">
@@ -15698,7 +15698,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H275" t="n">
@@ -15754,7 +15754,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H276" t="n">
@@ -15808,7 +15808,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H277" t="n">
@@ -15864,7 +15864,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H278" t="n">
@@ -15918,7 +15918,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H279" t="n">
@@ -15972,7 +15972,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H280" t="n">
@@ -16028,7 +16028,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H281" t="n">
@@ -16084,7 +16084,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H282" t="n">
@@ -16138,7 +16138,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H283" t="n">
@@ -16194,7 +16194,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H284" t="n">
@@ -16250,7 +16250,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H285" t="n">
@@ -16306,7 +16306,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H286" t="n">
@@ -16360,7 +16360,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H287" t="n">
@@ -16414,7 +16414,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H288" t="n">
@@ -16468,7 +16468,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H289" t="n">
@@ -16522,7 +16522,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H290" t="n">
@@ -16578,7 +16578,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H291" t="n">
@@ -16634,7 +16634,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H292" t="n">
@@ -16690,7 +16690,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H293" t="n">
@@ -16746,7 +16746,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H294" t="n">
@@ -16802,7 +16802,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H295" t="n">
@@ -16858,7 +16858,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H296" t="n">
@@ -16914,7 +16914,7 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H297" t="n">
@@ -16970,7 +16970,7 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H298" t="n">
@@ -17026,7 +17026,7 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H299" t="n">
@@ -17082,7 +17082,7 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H300" t="n">
@@ -17138,7 +17138,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H301" t="n">
@@ -17194,7 +17194,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H302" t="n">
@@ -17250,7 +17250,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H303" t="n">
@@ -17306,7 +17306,7 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H304" t="n">
@@ -17362,7 +17362,7 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H305" t="n">
@@ -17418,7 +17418,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H306" t="n">
@@ -17472,7 +17472,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H307" t="n">
@@ -17528,7 +17528,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H308" t="n">
@@ -17584,7 +17584,7 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H309" t="n">
@@ -17638,7 +17638,7 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H310" t="n">
@@ -17692,7 +17692,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H311" t="n">
@@ -17746,7 +17746,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H312" t="n">
@@ -17800,7 +17800,7 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H313" t="n">
@@ -17856,7 +17856,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H314" t="n">
@@ -17910,7 +17910,7 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H315" t="n">
@@ -18020,7 +18020,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H317" t="n">
@@ -18074,7 +18074,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H318" t="n">
@@ -18130,7 +18130,7 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H319" t="n">
@@ -18184,7 +18184,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H320" t="n">
@@ -18240,7 +18240,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H321" t="n">
@@ -18294,7 +18294,7 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H322" t="n">
@@ -18348,7 +18348,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H323" t="n">
@@ -18402,7 +18402,7 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H324" t="n">
@@ -18456,7 +18456,7 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H325" t="n">
@@ -18510,7 +18510,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H326" t="n">
@@ -18564,7 +18564,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H327" t="n">
@@ -18620,7 +18620,7 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H328" t="n">
@@ -18676,7 +18676,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H329" t="n">
@@ -18732,7 +18732,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H330" t="n">
@@ -18788,7 +18788,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H331" t="n">
@@ -18844,7 +18844,7 @@
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H332" t="n">
@@ -18900,7 +18900,7 @@
       </c>
       <c r="G333" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H333" t="n">
@@ -18956,7 +18956,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H334" t="n">
@@ -19012,7 +19012,7 @@
       </c>
       <c r="G335" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H335" t="n">
@@ -19066,7 +19066,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H336" t="n">
@@ -19122,7 +19122,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H337" t="n">
@@ -19176,7 +19176,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H338" t="n">
@@ -19230,7 +19230,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H339" t="n">
@@ -19284,7 +19284,7 @@
       </c>
       <c r="G340" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H340" t="n">
@@ -19340,7 +19340,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H341" t="n">
@@ -19394,7 +19394,7 @@
       </c>
       <c r="G342" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H342" t="n">
@@ -19448,7 +19448,7 @@
       </c>
       <c r="G343" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H343" t="n">
@@ -19502,7 +19502,7 @@
       </c>
       <c r="G344" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H344" t="n">
@@ -19558,7 +19558,7 @@
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H345" t="n">
@@ -19614,7 +19614,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H346" t="n">
@@ -19670,7 +19670,7 @@
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H347" t="n">
@@ -19724,7 +19724,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H348" t="n">
@@ -19778,7 +19778,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H349" t="n">
@@ -19832,7 +19832,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H350" t="n">
@@ -19886,7 +19886,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H351" t="n">
@@ -19940,7 +19940,7 @@
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H352" t="n">
@@ -19994,7 +19994,7 @@
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H353" t="n">
@@ -20048,7 +20048,7 @@
       </c>
       <c r="G354" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H354" t="n">
@@ -20102,7 +20102,7 @@
       </c>
       <c r="G355" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H355" t="n">
@@ -20156,7 +20156,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H356" t="n">
@@ -20210,7 +20210,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H357" t="n">
@@ -20264,7 +20264,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H358" t="n">
@@ -20318,7 +20318,7 @@
       </c>
       <c r="G359" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H359" t="n">
@@ -20372,7 +20372,7 @@
       </c>
       <c r="G360" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H360" t="n">
@@ -20428,7 +20428,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H361" t="n">
@@ -20484,7 +20484,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H362" t="n">
@@ -20540,7 +20540,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H363" t="n">
@@ -20596,7 +20596,7 @@
       </c>
       <c r="G364" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H364" t="n">
@@ -20650,7 +20650,7 @@
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H365" t="n">
@@ -20706,7 +20706,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H366" t="n">
@@ -20760,7 +20760,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H367" t="n">
@@ -20814,7 +20814,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H368" t="n">
@@ -20870,7 +20870,7 @@
       </c>
       <c r="G369" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H369" t="n">
@@ -20924,7 +20924,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H370" t="n">
@@ -20980,7 +20980,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H371" t="n">
@@ -21034,7 +21034,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H372" t="n">
@@ -21090,7 +21090,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H373" t="n">
@@ -21144,7 +21144,7 @@
       </c>
       <c r="G374" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H374" t="n">
@@ -21200,7 +21200,7 @@
       </c>
       <c r="G375" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H375" t="n">
@@ -21256,7 +21256,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H376" t="n">
@@ -21312,7 +21312,7 @@
       </c>
       <c r="G377" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H377" t="n">
@@ -21366,7 +21366,7 @@
       </c>
       <c r="G378" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H378" t="n">
@@ -21420,7 +21420,7 @@
       </c>
       <c r="G379" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H379" t="n">
@@ -21474,7 +21474,7 @@
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H380" t="n">
@@ -21528,7 +21528,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H381" t="n">
@@ -21582,7 +21582,7 @@
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H382" t="n">
@@ -21636,7 +21636,7 @@
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H383" t="n">
@@ -21690,7 +21690,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H384" t="n">
@@ -21746,7 +21746,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H385" t="n">
@@ -21802,7 +21802,7 @@
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H386" t="n">
@@ -21858,7 +21858,7 @@
       </c>
       <c r="G387" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H387" t="n">
@@ -21912,7 +21912,7 @@
       </c>
       <c r="G388" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H388" t="n">
@@ -21968,7 +21968,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H389" t="n">
@@ -22022,7 +22022,7 @@
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H390" t="n">
@@ -22076,7 +22076,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H391" t="n">
@@ -22130,7 +22130,7 @@
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H392" t="n">
@@ -22184,7 +22184,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H393" t="n">
@@ -22238,7 +22238,7 @@
       </c>
       <c r="G394" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H394" t="n">
@@ -22292,7 +22292,7 @@
       </c>
       <c r="G395" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H395" t="n">
@@ -22346,7 +22346,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H396" t="n">
@@ -22400,7 +22400,7 @@
       </c>
       <c r="G397" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H397" t="n">
@@ -22454,7 +22454,7 @@
       </c>
       <c r="G398" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H398" t="n">
@@ -22508,7 +22508,7 @@
       </c>
       <c r="G399" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H399" t="n">
@@ -22562,7 +22562,7 @@
       </c>
       <c r="G400" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H400" t="n">
@@ -22616,7 +22616,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H401" t="n">
@@ -22670,7 +22670,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H402" t="n">
@@ -22724,7 +22724,7 @@
       </c>
       <c r="G403" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H403" t="n">
@@ -22778,7 +22778,7 @@
       </c>
       <c r="G404" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H404" t="n">
@@ -22834,7 +22834,7 @@
       </c>
       <c r="G405" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H405" t="n">
@@ -22890,7 +22890,7 @@
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H406" t="n">
@@ -22946,7 +22946,7 @@
       </c>
       <c r="G407" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H407" t="n">
@@ -23002,7 +23002,7 @@
       </c>
       <c r="G408" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H408" t="n">
@@ -23056,7 +23056,7 @@
       </c>
       <c r="G409" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H409" t="n">
@@ -23110,7 +23110,7 @@
       </c>
       <c r="G410" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H410" t="n">
@@ -23166,7 +23166,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H411" t="n">
@@ -23220,7 +23220,7 @@
       </c>
       <c r="G412" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H412" t="n">
@@ -23274,7 +23274,7 @@
       </c>
       <c r="G413" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H413" t="n">
@@ -23328,7 +23328,7 @@
       </c>
       <c r="G414" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H414" t="n">
@@ -23382,7 +23382,7 @@
       </c>
       <c r="G415" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H415" t="n">
@@ -23436,7 +23436,7 @@
       </c>
       <c r="G416" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H416" t="n">
@@ -23492,7 +23492,7 @@
       </c>
       <c r="G417" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H417" t="n">
@@ -23548,7 +23548,7 @@
       </c>
       <c r="G418" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H418" t="n">
@@ -23602,7 +23602,7 @@
       </c>
       <c r="G419" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H419" t="n">
@@ -23656,7 +23656,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H420" t="n">
@@ -23712,7 +23712,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H421" t="n">
@@ -23768,7 +23768,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H422" t="n">
@@ -23822,7 +23822,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H423" t="n">
@@ -23876,7 +23876,7 @@
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H424" t="n">
@@ -23932,7 +23932,7 @@
       </c>
       <c r="G425" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H425" t="n">
@@ -23986,7 +23986,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H426" t="n">
@@ -24042,7 +24042,7 @@
       </c>
       <c r="G427" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H427" t="n">
@@ -24098,7 +24098,7 @@
       </c>
       <c r="G428" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H428" t="n">
@@ -24154,7 +24154,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H429" t="n">
@@ -24208,7 +24208,7 @@
       </c>
       <c r="G430" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H430" t="n">
@@ -24262,7 +24262,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H431" t="n">
@@ -24318,7 +24318,7 @@
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H432" t="n">
@@ -24374,7 +24374,7 @@
       </c>
       <c r="G433" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H433" t="n">
@@ -24430,7 +24430,7 @@
       </c>
       <c r="G434" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H434" t="n">
@@ -24486,7 +24486,7 @@
       </c>
       <c r="G435" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H435" t="n">
@@ -24542,7 +24542,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H436" t="n">
@@ -24596,7 +24596,7 @@
       </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H437" t="n">
@@ -24650,7 +24650,7 @@
       </c>
       <c r="G438" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H438" t="n">
@@ -24704,7 +24704,7 @@
       </c>
       <c r="G439" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H439" t="n">
@@ -24758,7 +24758,7 @@
       </c>
       <c r="G440" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H440" t="n">
@@ -24812,7 +24812,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H441" t="n">
@@ -24866,7 +24866,7 @@
       </c>
       <c r="G442" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H442" t="n">
@@ -24920,7 +24920,7 @@
       </c>
       <c r="G443" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H443" t="n">
@@ -24974,7 +24974,7 @@
       </c>
       <c r="G444" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H444" t="n">
@@ -25028,7 +25028,7 @@
       </c>
       <c r="G445" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H445" t="n">
@@ -25082,7 +25082,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H446" t="n">
@@ -25136,7 +25136,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H447" t="n">
@@ -25190,7 +25190,7 @@
       </c>
       <c r="G448" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H448" t="n">
@@ -25244,7 +25244,7 @@
       </c>
       <c r="G449" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H449" t="n">
@@ -25300,7 +25300,7 @@
       </c>
       <c r="G450" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H450" t="n">
@@ -25356,7 +25356,7 @@
       </c>
       <c r="G451" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H451" t="n">
@@ -25412,7 +25412,7 @@
       </c>
       <c r="G452" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H452" t="n">
@@ -25468,7 +25468,7 @@
       </c>
       <c r="G453" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H453" t="n">
@@ -25522,7 +25522,7 @@
       </c>
       <c r="G454" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H454" t="n">
@@ -25576,7 +25576,7 @@
       </c>
       <c r="G455" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H455" t="n">
@@ -25632,7 +25632,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H456" t="n">
@@ -25688,7 +25688,7 @@
       </c>
       <c r="G457" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H457" t="n">
@@ -25744,7 +25744,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H458" t="n">
@@ -25800,7 +25800,7 @@
       </c>
       <c r="G459" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H459" t="n">
@@ -25854,7 +25854,7 @@
       </c>
       <c r="G460" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H460" t="n">
@@ -25908,7 +25908,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H461" t="n">
@@ -25962,7 +25962,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H462" t="n">
@@ -26016,7 +26016,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H463" t="n">
@@ -26070,7 +26070,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H464" t="n">
@@ -26124,7 +26124,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H465" t="n">
@@ -26178,7 +26178,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H466" t="n">
@@ -26234,7 +26234,7 @@
       </c>
       <c r="G467" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H467" t="n">
@@ -26288,7 +26288,7 @@
       </c>
       <c r="G468" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H468" t="n">
@@ -26342,7 +26342,7 @@
       </c>
       <c r="G469" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H469" t="n">
@@ -26396,7 +26396,7 @@
       </c>
       <c r="G470" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H470" t="n">
@@ -26450,7 +26450,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H471" t="n">
@@ -26504,7 +26504,7 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H472" t="n">
@@ -26558,7 +26558,7 @@
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H473" t="n">
@@ -26614,7 +26614,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H474" t="n">
@@ -26670,7 +26670,7 @@
       </c>
       <c r="G475" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H475" t="n">
@@ -26726,7 +26726,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H476" t="n">
@@ -26782,7 +26782,7 @@
       </c>
       <c r="G477" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H477" t="n">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="G486" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>9000 100F / CC NEEDED</t>
         </is>
       </c>
       <c r="H486" t="n">
@@ -27358,22 +27358,12 @@
       <c r="D488" t="inlineStr"/>
       <c r="E488" t="inlineStr"/>
       <c r="F488" t="inlineStr"/>
-      <c r="G488" t="inlineStr">
-        <is>
-          <t>9000 100F</t>
-        </is>
-      </c>
+      <c r="G488" t="inlineStr"/>
       <c r="H488" t="inlineStr"/>
-      <c r="I488" t="n">
-        <v>0</v>
-      </c>
+      <c r="I488" t="inlineStr"/>
       <c r="J488" t="inlineStr"/>
-      <c r="K488" t="n">
-        <v>0</v>
-      </c>
-      <c r="L488" t="n">
-        <v>0</v>
-      </c>
+      <c r="K488" t="inlineStr"/>
+      <c r="L488" t="inlineStr"/>
       <c r="M488" t="inlineStr"/>
       <c r="N488" t="inlineStr"/>
       <c r="O488" t="inlineStr"/>
@@ -27386,11 +27376,7 @@
       <c r="D489" t="inlineStr"/>
       <c r="E489" t="inlineStr"/>
       <c r="F489" t="inlineStr"/>
-      <c r="G489" t="inlineStr">
-        <is>
-          <t>9000 100F</t>
-        </is>
-      </c>
+      <c r="G489" t="inlineStr"/>
       <c r="H489" t="inlineStr"/>
       <c r="I489" t="n">
         <v>243.1700000000002</v>

</xml_diff>

<commit_message>
Automate equipment billing by incorporating updates from allocation worksheets
Refactor billing process to use PM allocation revisions by adding `extract_pm_allocations.py` and modifying `process_pm_allocations.py` and `quick_billing_processor.py`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/335d2b2a-ba5e-4a1f-a007-d39583554736.jpg
</commit_message>
<xml_diff>
--- a/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
+++ b/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
@@ -440,62 +440,62 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>division</t>
+          <t>Division</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>equip_id</t>
+          <t>Equip #</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>Equipment Description</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>job</t>
+          <t>Job</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>phase</t>
+          <t>Phase</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>cost_code</t>
+          <t>Cost Code</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cost_class</t>
+          <t>Cost Class</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>units</t>
+          <t>Units</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>frequency</t>
+          <t>Frequency</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>rate</t>
+          <t>Rate</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>amount</t>
+          <t>Amount</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Improve billing data extraction and processing for more accurate reports
Refactors billing data processing across multiple files to incorporate PM allocations and improve data loading from RAGLE files using pandas.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/c9c3fc1d-1f0a-45d3-9938-86b706535be6.jpg
</commit_message>
<xml_diff>
--- a/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
+++ b/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
@@ -3598,7 +3598,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -3652,7 +3652,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -3706,7 +3706,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5538,7 +5538,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -5594,7 +5594,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -5654,7 +5654,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -5710,7 +5710,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -5770,7 +5770,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -5830,7 +5830,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -5890,7 +5890,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -5950,7 +5950,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -6006,7 +6006,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -6060,7 +6060,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -6114,7 +6114,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -6170,7 +6170,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -6226,7 +6226,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -6282,7 +6282,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -6338,7 +6338,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -6394,7 +6394,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -6450,7 +6450,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -6506,7 +6506,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -6562,7 +6562,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -6616,7 +6616,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -6670,7 +6670,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -6726,7 +6726,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -6782,7 +6782,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -6838,7 +6838,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -6892,7 +6892,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -6946,7 +6946,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -7002,7 +7002,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -7058,7 +7058,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -7114,7 +7114,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -7174,7 +7174,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -7230,7 +7230,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -7286,7 +7286,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -7340,7 +7340,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -7396,7 +7396,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -7452,7 +7452,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -7508,7 +7508,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -8396,7 +8396,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -8450,7 +8450,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>WT</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -14720,7 +14720,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -14780,7 +14780,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -14836,7 +14836,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -14892,7 +14892,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -14948,7 +14948,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -15004,7 +15004,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -15060,7 +15060,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -15116,7 +15116,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -15170,7 +15170,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -15226,7 +15226,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -15282,7 +15282,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -15336,7 +15336,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -15392,7 +15392,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -15448,7 +15448,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -15504,7 +15504,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -15560,7 +15560,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -15616,7 +15616,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -15672,7 +15672,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -15728,7 +15728,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -15782,7 +15782,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -15838,7 +15838,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -15892,7 +15892,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -21008,7 +21008,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -21064,7 +21064,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -21118,7 +21118,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -21174,7 +21174,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -21230,7 +21230,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -21286,7 +21286,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -21340,7 +21340,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -21394,7 +21394,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -21448,7 +21448,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -21502,7 +21502,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -21556,7 +21556,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -21610,7 +21610,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -21664,7 +21664,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -21720,7 +21720,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -23906,7 +23906,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -23960,7 +23960,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -24016,7 +24016,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -24072,7 +24072,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
@@ -24128,7 +24128,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
@@ -24182,7 +24182,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -24236,7 +24236,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -24292,7 +24292,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -24348,7 +24348,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -24404,7 +24404,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
@@ -24460,7 +24460,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -24786,7 +24786,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
@@ -24840,7 +24840,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
@@ -24894,7 +24894,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -24948,7 +24948,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -25002,7 +25002,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -25056,7 +25056,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -25110,7 +25110,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -25164,7 +25164,7 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
@@ -25218,7 +25218,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -25274,7 +25274,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -25330,7 +25330,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -25386,7 +25386,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -25442,7 +25442,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
@@ -25496,7 +25496,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
@@ -25550,7 +25550,7 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
@@ -25606,7 +25606,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -25662,7 +25662,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -25718,7 +25718,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -25774,7 +25774,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -25828,7 +25828,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -25882,7 +25882,7 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
@@ -25936,7 +25936,7 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
@@ -25990,7 +25990,7 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
@@ -26044,7 +26044,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -26098,7 +26098,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -26152,7 +26152,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -26208,7 +26208,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -26262,7 +26262,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -26316,7 +26316,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -26370,7 +26370,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -26424,7 +26424,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -26478,7 +26478,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -26532,7 +26532,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -26588,7 +26588,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -26644,7 +26644,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -26700,7 +26700,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>DFW</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -27352,7 +27352,11 @@
       <c r="P487" t="inlineStr"/>
     </row>
     <row r="488">
-      <c r="A488" t="inlineStr"/>
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>DFW</t>
+        </is>
+      </c>
       <c r="B488" t="inlineStr"/>
       <c r="C488" t="inlineStr"/>
       <c r="D488" t="inlineStr"/>
@@ -27370,7 +27374,11 @@
       <c r="P488" t="inlineStr"/>
     </row>
     <row r="489">
-      <c r="A489" t="inlineStr"/>
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>DFW</t>
+        </is>
+      </c>
       <c r="B489" t="inlineStr"/>
       <c r="C489" t="inlineStr"/>
       <c r="D489" t="inlineStr"/>

</xml_diff>

<commit_message>
Apply PM-reviewed unit allocations to generate accurate billing amounts
Recalculates billing amounts by applying PM-provided unit allocations from allocation sheets, ignoring base file totals.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/c9c3fc1d-1f0a-45d3-9938-86b706535be6.jpg
</commit_message>
<xml_diff>
--- a/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
+++ b/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
@@ -3598,7 +3598,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -3652,7 +3652,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -3706,7 +3706,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5538,7 +5538,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -5564,7 +5564,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H92" t="n">
@@ -5594,7 +5594,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -5620,7 +5620,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H93" t="n">
@@ -5654,7 +5654,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -5680,7 +5680,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -5710,7 +5710,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -5736,7 +5736,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H95" t="n">
@@ -5770,7 +5770,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -5796,7 +5796,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H96" t="n">
@@ -5830,7 +5830,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -5856,7 +5856,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H97" t="n">
@@ -5890,7 +5890,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -5916,7 +5916,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H98" t="n">
@@ -5950,7 +5950,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -6006,7 +6006,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -6060,7 +6060,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -6114,7 +6114,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -6170,7 +6170,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -6226,7 +6226,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -6282,7 +6282,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H105" t="n">
@@ -6338,7 +6338,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -6364,7 +6364,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H106" t="n">
@@ -6394,7 +6394,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -6420,7 +6420,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H107" t="n">
@@ -6450,7 +6450,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H108" t="n">
@@ -6506,7 +6506,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H109" t="n">
@@ -6562,7 +6562,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -6616,7 +6616,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -6670,7 +6670,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -6726,7 +6726,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -6782,7 +6782,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -6808,7 +6808,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H114" t="n">
@@ -6838,7 +6838,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -6892,7 +6892,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -6946,7 +6946,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -6972,7 +6972,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H117" t="n">
@@ -7002,7 +7002,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H118" t="n">
@@ -7058,7 +7058,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H119" t="n">
@@ -7114,7 +7114,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -7140,7 +7140,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H120" t="n">
@@ -7174,7 +7174,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -7200,7 +7200,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>9000 100M | 9000 100F | CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H121" t="n">
@@ -7230,7 +7230,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -7286,7 +7286,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -7312,7 +7312,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>9000 100M | 9000 100F | CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H123" t="n">
@@ -7340,7 +7340,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -7366,7 +7366,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H124" t="n">
@@ -7396,7 +7396,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H125" t="n">
@@ -7452,7 +7452,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H126" t="n">
@@ -7508,7 +7508,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -7534,7 +7534,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H127" t="n">
@@ -8396,7 +8396,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H143" t="n">
@@ -8450,7 +8450,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>WT</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -8476,7 +8476,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H144" t="n">
@@ -8532,7 +8532,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H145" t="n">
@@ -8588,7 +8588,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H146" t="n">
@@ -8644,7 +8644,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H147" t="n">
@@ -8700,7 +8700,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H148" t="n">
@@ -8756,7 +8756,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H149" t="n">
@@ -8812,7 +8812,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H150" t="n">
@@ -8868,7 +8868,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H151" t="n">
@@ -8924,7 +8924,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H152" t="n">
@@ -8980,7 +8980,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H153" t="n">
@@ -9036,7 +9036,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H154" t="n">
@@ -9092,7 +9092,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H155" t="n">
@@ -9146,7 +9146,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H156" t="n">
@@ -9202,7 +9202,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H157" t="n">
@@ -9258,7 +9258,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H158" t="n">
@@ -9314,7 +9314,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H159" t="n">
@@ -9368,7 +9368,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H160" t="n">
@@ -9424,7 +9424,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H161" t="n">
@@ -9480,7 +9480,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H162" t="n">
@@ -9536,7 +9536,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H163" t="n">
@@ -9592,7 +9592,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H164" t="n">
@@ -9648,7 +9648,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H165" t="n">
@@ -9704,7 +9704,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H166" t="n">
@@ -9760,7 +9760,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H167" t="n">
@@ -9816,7 +9816,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H168" t="n">
@@ -9872,7 +9872,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H169" t="n">
@@ -9928,7 +9928,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H170" t="n">
@@ -9984,7 +9984,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H171" t="n">
@@ -10040,7 +10040,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H172" t="n">
@@ -10096,7 +10096,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H173" t="n">
@@ -10152,7 +10152,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H174" t="n">
@@ -10208,7 +10208,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H175" t="n">
@@ -10264,7 +10264,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H176" t="n">
@@ -10320,7 +10320,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H177" t="n">
@@ -10376,7 +10376,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H178" t="n">
@@ -10484,7 +10484,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H180" t="n">
@@ -10538,7 +10538,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H181" t="n">
@@ -10594,7 +10594,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H182" t="n">
@@ -10650,7 +10650,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H183" t="n">
@@ -10706,7 +10706,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H184" t="n">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H185" t="n">
@@ -10818,7 +10818,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H186" t="n">
@@ -10872,7 +10872,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H187" t="n">
@@ -10926,7 +10926,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H188" t="n">
@@ -10980,7 +10980,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H189" t="n">
@@ -11036,7 +11036,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H190" t="n">
@@ -11090,7 +11090,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H191" t="n">
@@ -11146,7 +11146,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H192" t="n">
@@ -11202,7 +11202,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H193" t="n">
@@ -11256,7 +11256,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H194" t="n">
@@ -11310,7 +11310,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H195" t="n">
@@ -11364,7 +11364,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H196" t="n">
@@ -11420,7 +11420,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H197" t="n">
@@ -11476,7 +11476,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H198" t="n">
@@ -11532,7 +11532,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H199" t="n">
@@ -11588,7 +11588,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H200" t="n">
@@ -11644,7 +11644,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H201" t="n">
@@ -11700,7 +11700,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H202" t="n">
@@ -11812,7 +11812,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H204" t="n">
@@ -11866,7 +11866,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H205" t="n">
@@ -11922,7 +11922,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H206" t="n">
@@ -11978,7 +11978,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H207" t="n">
@@ -12034,7 +12034,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H208" t="n">
@@ -12090,7 +12090,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H209" t="n">
@@ -12146,7 +12146,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H210" t="n">
@@ -12202,7 +12202,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H211" t="n">
@@ -12258,7 +12258,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H212" t="n">
@@ -12312,7 +12312,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H213" t="n">
@@ -12366,7 +12366,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H214" t="n">
@@ -12420,7 +12420,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H215" t="n">
@@ -12474,7 +12474,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H216" t="n">
@@ -12528,7 +12528,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H217" t="n">
@@ -12582,7 +12582,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H218" t="n">
@@ -12636,7 +12636,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H219" t="n">
@@ -12690,7 +12690,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H220" t="n">
@@ -12744,7 +12744,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H221" t="n">
@@ -12798,7 +12798,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H222" t="n">
@@ -12852,7 +12852,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H223" t="n">
@@ -12906,7 +12906,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H224" t="n">
@@ -12960,7 +12960,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H225" t="n">
@@ -13014,7 +13014,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H226" t="n">
@@ -13068,7 +13068,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H227" t="n">
@@ -13122,7 +13122,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H228" t="n">
@@ -13176,7 +13176,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H229" t="n">
@@ -13230,7 +13230,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H230" t="n">
@@ -13284,7 +13284,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H231" t="n">
@@ -13338,7 +13338,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H232" t="n">
@@ -13392,7 +13392,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H233" t="n">
@@ -13446,7 +13446,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H234" t="n">
@@ -13500,7 +13500,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H235" t="n">
@@ -13556,7 +13556,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H236" t="n">
@@ -13610,7 +13610,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H237" t="n">
@@ -13664,7 +13664,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H238" t="n">
@@ -13718,7 +13718,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H239" t="n">
@@ -13772,7 +13772,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H240" t="n">
@@ -13828,7 +13828,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H241" t="n">
@@ -13882,7 +13882,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H242" t="n">
@@ -13936,7 +13936,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H243" t="n">
@@ -13990,7 +13990,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H244" t="n">
@@ -14044,7 +14044,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H245" t="n">
@@ -14098,7 +14098,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H246" t="n">
@@ -14152,7 +14152,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H247" t="n">
@@ -14206,7 +14206,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H248" t="n">
@@ -14260,7 +14260,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H249" t="n">
@@ -14314,7 +14314,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H250" t="n">
@@ -14368,7 +14368,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H251" t="n">
@@ -14422,7 +14422,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H252" t="n">
@@ -14476,7 +14476,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H253" t="n">
@@ -14584,7 +14584,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H255" t="n">
@@ -14638,7 +14638,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H256" t="n">
@@ -14692,7 +14692,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H257" t="n">
@@ -14720,7 +14720,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -14746,7 +14746,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H258" t="n">
@@ -14780,7 +14780,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -14806,7 +14806,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H259" t="n">
@@ -14836,7 +14836,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -14862,7 +14862,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H260" t="n">
@@ -14892,7 +14892,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -14918,7 +14918,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H261" t="n">
@@ -14948,7 +14948,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -14974,7 +14974,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H262" t="n">
@@ -15004,7 +15004,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -15030,7 +15030,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H263" t="n">
@@ -15060,7 +15060,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -15086,7 +15086,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H264" t="n">
@@ -15116,7 +15116,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -15142,7 +15142,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H265" t="n">
@@ -15170,7 +15170,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -15196,7 +15196,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H266" t="n">
@@ -15226,7 +15226,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -15252,7 +15252,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H267" t="n">
@@ -15282,7 +15282,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -15308,7 +15308,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H268" t="n">
@@ -15336,7 +15336,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -15362,7 +15362,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H269" t="n">
@@ -15392,7 +15392,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -15418,7 +15418,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H270" t="n">
@@ -15448,7 +15448,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -15474,7 +15474,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H271" t="n">
@@ -15504,7 +15504,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -15530,7 +15530,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H272" t="n">
@@ -15560,7 +15560,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -15586,7 +15586,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H273" t="n">
@@ -15616,7 +15616,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -15642,7 +15642,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H274" t="n">
@@ -15672,7 +15672,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -15698,7 +15698,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H275" t="n">
@@ -15728,7 +15728,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -15754,7 +15754,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H276" t="n">
@@ -15782,7 +15782,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -15808,7 +15808,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H277" t="n">
@@ -15838,7 +15838,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -15864,7 +15864,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H278" t="n">
@@ -15892,7 +15892,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -15918,7 +15918,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H279" t="n">
@@ -15972,7 +15972,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H280" t="n">
@@ -16028,7 +16028,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H281" t="n">
@@ -16084,7 +16084,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H282" t="n">
@@ -16138,7 +16138,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H283" t="n">
@@ -16194,7 +16194,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H284" t="n">
@@ -16250,7 +16250,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H285" t="n">
@@ -16306,7 +16306,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H286" t="n">
@@ -16360,7 +16360,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H287" t="n">
@@ -16414,7 +16414,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H288" t="n">
@@ -16468,7 +16468,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H289" t="n">
@@ -16522,7 +16522,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H290" t="n">
@@ -16578,7 +16578,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H291" t="n">
@@ -16634,7 +16634,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100M</t>
         </is>
       </c>
       <c r="H292" t="n">
@@ -16690,7 +16690,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H293" t="n">
@@ -16746,7 +16746,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H294" t="n">
@@ -16802,7 +16802,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H295" t="n">
@@ -16858,7 +16858,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H296" t="n">
@@ -16914,7 +16914,7 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H297" t="n">
@@ -16970,7 +16970,7 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H298" t="n">
@@ -17026,7 +17026,7 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H299" t="n">
@@ -17082,7 +17082,7 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H300" t="n">
@@ -17138,7 +17138,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H301" t="n">
@@ -17194,7 +17194,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H302" t="n">
@@ -17250,7 +17250,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H303" t="n">
@@ -17306,7 +17306,7 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H304" t="n">
@@ -17362,7 +17362,7 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H305" t="n">
@@ -17418,7 +17418,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H306" t="n">
@@ -17472,7 +17472,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H307" t="n">
@@ -17528,7 +17528,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H308" t="n">
@@ -17584,7 +17584,7 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H309" t="n">
@@ -17638,7 +17638,7 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H310" t="n">
@@ -17746,7 +17746,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H312" t="n">
@@ -17800,7 +17800,7 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H313" t="n">
@@ -17856,7 +17856,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H314" t="n">
@@ -17910,7 +17910,7 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H315" t="n">
@@ -17966,7 +17966,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H316" t="n">
@@ -18020,7 +18020,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H317" t="n">
@@ -18074,7 +18074,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H318" t="n">
@@ -18130,7 +18130,7 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H319" t="n">
@@ -18184,7 +18184,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H320" t="n">
@@ -18240,7 +18240,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H321" t="n">
@@ -18294,7 +18294,7 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H322" t="n">
@@ -18348,7 +18348,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H323" t="n">
@@ -18402,7 +18402,7 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H324" t="n">
@@ -18456,7 +18456,7 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H325" t="n">
@@ -18510,7 +18510,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H326" t="n">
@@ -18564,7 +18564,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H327" t="n">
@@ -18620,7 +18620,7 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H328" t="n">
@@ -18676,7 +18676,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H329" t="n">
@@ -18732,7 +18732,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H330" t="n">
@@ -18788,7 +18788,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H331" t="n">
@@ -18844,7 +18844,7 @@
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H332" t="n">
@@ -18900,7 +18900,7 @@
       </c>
       <c r="G333" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H333" t="n">
@@ -18956,7 +18956,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H334" t="n">
@@ -19012,7 +19012,7 @@
       </c>
       <c r="G335" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H335" t="n">
@@ -19066,7 +19066,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H336" t="n">
@@ -19122,7 +19122,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H337" t="n">
@@ -19176,7 +19176,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H338" t="n">
@@ -19230,7 +19230,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H339" t="n">
@@ -19284,7 +19284,7 @@
       </c>
       <c r="G340" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H340" t="n">
@@ -19340,7 +19340,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H341" t="n">
@@ -19394,7 +19394,7 @@
       </c>
       <c r="G342" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H342" t="n">
@@ -19448,7 +19448,7 @@
       </c>
       <c r="G343" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H343" t="n">
@@ -19502,7 +19502,7 @@
       </c>
       <c r="G344" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H344" t="n">
@@ -19558,7 +19558,7 @@
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H345" t="n">
@@ -19614,7 +19614,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H346" t="n">
@@ -19670,7 +19670,7 @@
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H347" t="n">
@@ -19724,7 +19724,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H348" t="n">
@@ -19778,7 +19778,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H349" t="n">
@@ -19832,7 +19832,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H350" t="n">
@@ -19886,7 +19886,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H351" t="n">
@@ -19940,7 +19940,7 @@
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H352" t="n">
@@ -19994,7 +19994,7 @@
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H353" t="n">
@@ -20048,7 +20048,7 @@
       </c>
       <c r="G354" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H354" t="n">
@@ -20102,7 +20102,7 @@
       </c>
       <c r="G355" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H355" t="n">
@@ -20156,7 +20156,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H356" t="n">
@@ -20210,7 +20210,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H357" t="n">
@@ -20264,7 +20264,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H358" t="n">
@@ -20318,7 +20318,7 @@
       </c>
       <c r="G359" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H359" t="n">
@@ -20372,7 +20372,7 @@
       </c>
       <c r="G360" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H360" t="n">
@@ -20428,7 +20428,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H361" t="n">
@@ -20484,7 +20484,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H362" t="n">
@@ -20540,7 +20540,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H363" t="n">
@@ -20596,7 +20596,7 @@
       </c>
       <c r="G364" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H364" t="n">
@@ -20650,7 +20650,7 @@
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H365" t="n">
@@ -20760,7 +20760,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H367" t="n">
@@ -20814,7 +20814,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H368" t="n">
@@ -20870,7 +20870,7 @@
       </c>
       <c r="G369" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H369" t="n">
@@ -20924,7 +20924,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H370" t="n">
@@ -20980,7 +20980,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H371" t="n">
@@ -21008,7 +21008,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -21034,7 +21034,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H372" t="n">
@@ -21064,7 +21064,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -21090,7 +21090,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H373" t="n">
@@ -21118,7 +21118,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -21144,7 +21144,7 @@
       </c>
       <c r="G374" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H374" t="n">
@@ -21174,7 +21174,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -21200,7 +21200,7 @@
       </c>
       <c r="G375" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H375" t="n">
@@ -21230,7 +21230,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -21256,7 +21256,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H376" t="n">
@@ -21286,7 +21286,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -21312,7 +21312,7 @@
       </c>
       <c r="G377" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H377" t="n">
@@ -21340,7 +21340,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -21366,7 +21366,7 @@
       </c>
       <c r="G378" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H378" t="n">
@@ -21394,7 +21394,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -21420,7 +21420,7 @@
       </c>
       <c r="G379" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H379" t="n">
@@ -21448,7 +21448,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -21474,7 +21474,7 @@
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H380" t="n">
@@ -21502,7 +21502,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -21528,7 +21528,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H381" t="n">
@@ -21556,7 +21556,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -21582,7 +21582,7 @@
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H382" t="n">
@@ -21610,7 +21610,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -21636,7 +21636,7 @@
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H383" t="n">
@@ -21664,7 +21664,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -21690,7 +21690,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H384" t="n">
@@ -21720,7 +21720,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -21746,7 +21746,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H385" t="n">
@@ -21802,7 +21802,7 @@
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H386" t="n">
@@ -21858,7 +21858,7 @@
       </c>
       <c r="G387" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H387" t="n">
@@ -21912,7 +21912,7 @@
       </c>
       <c r="G388" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H388" t="n">
@@ -21968,7 +21968,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H389" t="n">
@@ -22022,7 +22022,7 @@
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H390" t="n">
@@ -22076,7 +22076,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H391" t="n">
@@ -22130,7 +22130,7 @@
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H392" t="n">
@@ -22184,7 +22184,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H393" t="n">
@@ -22238,7 +22238,7 @@
       </c>
       <c r="G394" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H394" t="n">
@@ -22292,7 +22292,7 @@
       </c>
       <c r="G395" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H395" t="n">
@@ -22346,7 +22346,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H396" t="n">
@@ -22400,7 +22400,7 @@
       </c>
       <c r="G397" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H397" t="n">
@@ -22454,7 +22454,7 @@
       </c>
       <c r="G398" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H398" t="n">
@@ -22508,7 +22508,7 @@
       </c>
       <c r="G399" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H399" t="n">
@@ -22562,7 +22562,7 @@
       </c>
       <c r="G400" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H400" t="n">
@@ -22616,7 +22616,7 @@
       </c>
       <c r="G401" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H401" t="n">
@@ -22670,7 +22670,7 @@
       </c>
       <c r="G402" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H402" t="n">
@@ -22724,7 +22724,7 @@
       </c>
       <c r="G403" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H403" t="n">
@@ -22778,7 +22778,7 @@
       </c>
       <c r="G404" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H404" t="n">
@@ -22834,7 +22834,7 @@
       </c>
       <c r="G405" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H405" t="n">
@@ -22890,7 +22890,7 @@
       </c>
       <c r="G406" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H406" t="n">
@@ -22946,7 +22946,7 @@
       </c>
       <c r="G407" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H407" t="n">
@@ -23002,7 +23002,7 @@
       </c>
       <c r="G408" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H408" t="n">
@@ -23056,7 +23056,7 @@
       </c>
       <c r="G409" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H409" t="n">
@@ -23110,7 +23110,7 @@
       </c>
       <c r="G410" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H410" t="n">
@@ -23166,7 +23166,7 @@
       </c>
       <c r="G411" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H411" t="n">
@@ -23220,7 +23220,7 @@
       </c>
       <c r="G412" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H412" t="n">
@@ -23274,7 +23274,7 @@
       </c>
       <c r="G413" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H413" t="n">
@@ -23328,7 +23328,7 @@
       </c>
       <c r="G414" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H414" t="n">
@@ -23382,7 +23382,7 @@
       </c>
       <c r="G415" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H415" t="n">
@@ -23436,7 +23436,7 @@
       </c>
       <c r="G416" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H416" t="n">
@@ -23492,7 +23492,7 @@
       </c>
       <c r="G417" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H417" t="n">
@@ -23548,7 +23548,7 @@
       </c>
       <c r="G418" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H418" t="n">
@@ -23602,7 +23602,7 @@
       </c>
       <c r="G419" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H419" t="n">
@@ -23656,7 +23656,7 @@
       </c>
       <c r="G420" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H420" t="n">
@@ -23712,7 +23712,7 @@
       </c>
       <c r="G421" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H421" t="n">
@@ -23768,7 +23768,7 @@
       </c>
       <c r="G422" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H422" t="n">
@@ -23822,7 +23822,7 @@
       </c>
       <c r="G423" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H423" t="n">
@@ -23876,7 +23876,7 @@
       </c>
       <c r="G424" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H424" t="n">
@@ -23906,7 +23906,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -23932,7 +23932,7 @@
       </c>
       <c r="G425" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H425" t="n">
@@ -23960,7 +23960,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -23986,7 +23986,7 @@
       </c>
       <c r="G426" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H426" t="n">
@@ -24016,7 +24016,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -24042,7 +24042,7 @@
       </c>
       <c r="G427" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H427" t="n">
@@ -24072,7 +24072,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
@@ -24098,7 +24098,7 @@
       </c>
       <c r="G428" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H428" t="n">
@@ -24128,7 +24128,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
@@ -24154,7 +24154,7 @@
       </c>
       <c r="G429" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H429" t="n">
@@ -24182,7 +24182,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -24208,7 +24208,7 @@
       </c>
       <c r="G430" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H430" t="n">
@@ -24236,7 +24236,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -24262,7 +24262,7 @@
       </c>
       <c r="G431" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H431" t="n">
@@ -24292,7 +24292,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -24318,7 +24318,7 @@
       </c>
       <c r="G432" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H432" t="n">
@@ -24348,7 +24348,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -24374,7 +24374,7 @@
       </c>
       <c r="G433" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H433" t="n">
@@ -24404,7 +24404,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
@@ -24430,7 +24430,7 @@
       </c>
       <c r="G434" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H434" t="n">
@@ -24460,7 +24460,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -24486,7 +24486,7 @@
       </c>
       <c r="G435" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H435" t="n">
@@ -24542,7 +24542,7 @@
       </c>
       <c r="G436" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H436" t="n">
@@ -24596,7 +24596,7 @@
       </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H437" t="n">
@@ -24650,7 +24650,7 @@
       </c>
       <c r="G438" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H438" t="n">
@@ -24704,7 +24704,7 @@
       </c>
       <c r="G439" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H439" t="n">
@@ -24758,7 +24758,7 @@
       </c>
       <c r="G440" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H440" t="n">
@@ -24786,7 +24786,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
@@ -24812,7 +24812,7 @@
       </c>
       <c r="G441" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H441" t="n">
@@ -24840,7 +24840,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
@@ -24866,7 +24866,7 @@
       </c>
       <c r="G442" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H442" t="n">
@@ -24894,7 +24894,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -24920,7 +24920,7 @@
       </c>
       <c r="G443" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H443" t="n">
@@ -24948,7 +24948,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -24974,7 +24974,7 @@
       </c>
       <c r="G444" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H444" t="n">
@@ -25002,7 +25002,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -25028,7 +25028,7 @@
       </c>
       <c r="G445" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H445" t="n">
@@ -25056,7 +25056,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -25082,7 +25082,7 @@
       </c>
       <c r="G446" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H446" t="n">
@@ -25110,7 +25110,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -25136,7 +25136,7 @@
       </c>
       <c r="G447" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H447" t="n">
@@ -25164,7 +25164,7 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
@@ -25190,7 +25190,7 @@
       </c>
       <c r="G448" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H448" t="n">
@@ -25218,7 +25218,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -25244,7 +25244,7 @@
       </c>
       <c r="G449" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H449" t="n">
@@ -25274,7 +25274,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -25300,7 +25300,7 @@
       </c>
       <c r="G450" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H450" t="n">
@@ -25330,7 +25330,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -25356,7 +25356,7 @@
       </c>
       <c r="G451" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H451" t="n">
@@ -25386,7 +25386,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -25412,7 +25412,7 @@
       </c>
       <c r="G452" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H452" t="n">
@@ -25442,7 +25442,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
@@ -25468,7 +25468,7 @@
       </c>
       <c r="G453" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H453" t="n">
@@ -25496,7 +25496,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
@@ -25522,7 +25522,7 @@
       </c>
       <c r="G454" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H454" t="n">
@@ -25550,7 +25550,7 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
@@ -25576,7 +25576,7 @@
       </c>
       <c r="G455" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H455" t="n">
@@ -25606,7 +25606,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -25632,7 +25632,7 @@
       </c>
       <c r="G456" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H456" t="n">
@@ -25662,7 +25662,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -25688,7 +25688,7 @@
       </c>
       <c r="G457" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H457" t="n">
@@ -25718,7 +25718,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -25744,7 +25744,7 @@
       </c>
       <c r="G458" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H458" t="n">
@@ -25774,7 +25774,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -25828,7 +25828,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -25854,7 +25854,7 @@
       </c>
       <c r="G460" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H460" t="n">
@@ -25882,7 +25882,7 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
@@ -25908,7 +25908,7 @@
       </c>
       <c r="G461" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H461" t="n">
@@ -25936,7 +25936,7 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
@@ -25962,7 +25962,7 @@
       </c>
       <c r="G462" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H462" t="n">
@@ -25990,7 +25990,7 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
@@ -26016,7 +26016,7 @@
       </c>
       <c r="G463" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H463" t="n">
@@ -26044,7 +26044,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -26070,7 +26070,7 @@
       </c>
       <c r="G464" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H464" t="n">
@@ -26098,7 +26098,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -26124,7 +26124,7 @@
       </c>
       <c r="G465" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H465" t="n">
@@ -26152,7 +26152,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -26178,7 +26178,7 @@
       </c>
       <c r="G466" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H466" t="n">
@@ -26208,7 +26208,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -26234,7 +26234,7 @@
       </c>
       <c r="G467" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H467" t="n">
@@ -26262,7 +26262,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -26288,7 +26288,7 @@
       </c>
       <c r="G468" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H468" t="n">
@@ -26316,7 +26316,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -26342,7 +26342,7 @@
       </c>
       <c r="G469" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H469" t="n">
@@ -26370,7 +26370,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -26396,7 +26396,7 @@
       </c>
       <c r="G470" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H470" t="n">
@@ -26424,7 +26424,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -26450,7 +26450,7 @@
       </c>
       <c r="G471" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H471" t="n">
@@ -26478,7 +26478,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -26504,7 +26504,7 @@
       </c>
       <c r="G472" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H472" t="n">
@@ -26532,7 +26532,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -26558,7 +26558,7 @@
       </c>
       <c r="G473" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H473" t="n">
@@ -26588,7 +26588,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -26614,7 +26614,7 @@
       </c>
       <c r="G474" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H474" t="n">
@@ -26644,7 +26644,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -26670,7 +26670,7 @@
       </c>
       <c r="G475" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H475" t="n">
@@ -26700,7 +26700,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>DFW</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -26726,7 +26726,7 @@
       </c>
       <c r="G476" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H476" t="n">
@@ -26782,7 +26782,7 @@
       </c>
       <c r="G477" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H477" t="n">
@@ -26998,7 +26998,7 @@
       </c>
       <c r="G481" t="inlineStr">
         <is>
-          <t>104 6001A</t>
+          <t>100 6002A</t>
         </is>
       </c>
       <c r="H481" t="n">
@@ -27054,7 +27054,7 @@
       </c>
       <c r="G482" t="inlineStr">
         <is>
-          <t>104 6001A</t>
+          <t>100 6002A</t>
         </is>
       </c>
       <c r="H482" t="n">
@@ -27162,7 +27162,7 @@
       </c>
       <c r="G484" t="inlineStr">
         <is>
-          <t>100 6002A</t>
+          <t>104 6001A</t>
         </is>
       </c>
       <c r="H484" t="n">
@@ -27272,7 +27272,7 @@
       </c>
       <c r="G486" t="inlineStr">
         <is>
-          <t>9000 100F / CC NEEDED</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H486" t="n">
@@ -27352,11 +27352,7 @@
       <c r="P487" t="inlineStr"/>
     </row>
     <row r="488">
-      <c r="A488" t="inlineStr">
-        <is>
-          <t>DFW</t>
-        </is>
-      </c>
+      <c r="A488" t="inlineStr"/>
       <c r="B488" t="inlineStr"/>
       <c r="C488" t="inlineStr"/>
       <c r="D488" t="inlineStr"/>
@@ -27374,11 +27370,7 @@
       <c r="P488" t="inlineStr"/>
     </row>
     <row r="489">
-      <c r="A489" t="inlineStr">
-        <is>
-          <t>DFW</t>
-        </is>
-      </c>
+      <c r="A489" t="inlineStr"/>
       <c r="B489" t="inlineStr"/>
       <c r="C489" t="inlineStr"/>
       <c r="D489" t="inlineStr"/>

</xml_diff>

<commit_message>
Update equipment codes and include the 0.5 revision unit allocation
Adjusts equipment codes and incorporates billing allocation file with 0.5 revision.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/e7530317-bd97-4746-a7d6-903dc88df70d.jpg
</commit_message>
<xml_diff>
--- a/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
+++ b/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
@@ -5620,7 +5620,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H93" t="n">
@@ -5680,7 +5680,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H94" t="n">
@@ -6086,7 +6086,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H101" t="n">
@@ -6140,7 +6140,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H102" t="n">
@@ -6196,7 +6196,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H103" t="n">
@@ -6252,7 +6252,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H104" t="n">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H105" t="n">
@@ -6364,7 +6364,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H106" t="n">
@@ -6420,7 +6420,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H107" t="n">
@@ -6476,7 +6476,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H108" t="n">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H109" t="n">
@@ -6642,7 +6642,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H111" t="n">
@@ -6696,7 +6696,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H112" t="n">
@@ -6752,7 +6752,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H113" t="n">
@@ -6918,7 +6918,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H116" t="n">
@@ -6972,7 +6972,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H117" t="n">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H118" t="n">
@@ -7084,7 +7084,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H119" t="n">
@@ -7312,7 +7312,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H123" t="n">
@@ -7366,7 +7366,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H124" t="n">
@@ -7422,7 +7422,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H125" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H126" t="n">
@@ -7534,7 +7534,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H127" t="n">
@@ -8422,7 +8422,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>9000 100M</t>
+          <t>9000 100F</t>
         </is>
       </c>
       <c r="H143" t="n">
@@ -12744,7 +12744,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6001 6002A</t>
         </is>
       </c>
       <c r="H221" t="n">
@@ -12798,7 +12798,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6001 6002A</t>
         </is>
       </c>
       <c r="H222" t="n">
@@ -14260,7 +14260,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6185 6002A</t>
         </is>
       </c>
       <c r="H249" t="n">
@@ -14314,7 +14314,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6185 6002A</t>
         </is>
       </c>
       <c r="H250" t="n">
@@ -14368,7 +14368,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6185 6002A</t>
         </is>
       </c>
       <c r="H251" t="n">
@@ -14422,7 +14422,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6185 6002A</t>
         </is>
       </c>
       <c r="H252" t="n">
@@ -14476,7 +14476,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6185 6002A</t>
         </is>
       </c>
       <c r="H253" t="n">
@@ -14584,7 +14584,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>9000 100F</t>
+          <t>6185 6002A</t>
         </is>
       </c>
       <c r="H255" t="n">

</xml_diff>

<commit_message>
Improve billing accuracy by prioritizing revisions over original units
Enhance final_billing_processor.py to prioritize 'Revision' column values over 'Units' where available, ensuring more precise billing data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: b83b866c-5b8f-4d82-9fde-612e7a355315
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/f2699832-8135-4557-9ec0-8d4d723b9ba2/e7530317-bd97-4746-a7d6-903dc88df70d.jpg
</commit_message>
<xml_diff>
--- a/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
+++ b/exports/FINALIZED_MASTER_ALLOCATION_SHEET_APRIL_2025.xlsx
@@ -12265,7 +12265,7 @@
         <v>4</v>
       </c>
       <c r="I212" t="n">
-        <v>0.04</v>
+        <v>0.5</v>
       </c>
       <c r="J212" t="inlineStr">
         <is>
@@ -12276,7 +12276,7 @@
         <v>200</v>
       </c>
       <c r="L212" t="n">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="M212" t="inlineStr"/>
       <c r="N212" t="inlineStr"/>
@@ -12319,7 +12319,7 @@
         <v>4</v>
       </c>
       <c r="I213" t="n">
-        <v>0.06</v>
+        <v>0.5</v>
       </c>
       <c r="J213" t="inlineStr">
         <is>
@@ -12330,7 +12330,7 @@
         <v>800</v>
       </c>
       <c r="L213" t="n">
-        <v>48</v>
+        <v>400</v>
       </c>
       <c r="M213" t="inlineStr"/>
       <c r="N213" t="inlineStr"/>
@@ -12373,7 +12373,7 @@
         <v>4</v>
       </c>
       <c r="I214" t="n">
-        <v>0.04</v>
+        <v>0.5</v>
       </c>
       <c r="J214" t="inlineStr">
         <is>
@@ -12384,7 +12384,7 @@
         <v>800</v>
       </c>
       <c r="L214" t="n">
-        <v>32</v>
+        <v>400</v>
       </c>
       <c r="M214" t="inlineStr"/>
       <c r="N214" t="inlineStr"/>
@@ -12427,7 +12427,7 @@
         <v>4</v>
       </c>
       <c r="I215" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -12438,7 +12438,7 @@
         <v>1200</v>
       </c>
       <c r="L215" t="n">
-        <v>84.00000000000001</v>
+        <v>600</v>
       </c>
       <c r="M215" t="inlineStr"/>
       <c r="N215" t="inlineStr"/>
@@ -14699,7 +14699,7 @@
         <v>4</v>
       </c>
       <c r="I257" t="n">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J257" t="inlineStr">
         <is>
@@ -14710,7 +14710,7 @@
         <v>3000</v>
       </c>
       <c r="L257" t="n">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="M257" t="inlineStr"/>
       <c r="N257" t="inlineStr"/>

</xml_diff>